<commit_message>
--excel data cleaning and update
</commit_message>
<xml_diff>
--- a/Pakaasa.xlsx
+++ b/Pakaasa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\paakasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99094B-841A-4DE9-97A5-ADAD01575245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935DDE2A-3D28-43E0-8370-90C6F701C5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="pakaasa" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pakaasa!$A$1:$AE$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pakaasa!$A$1:$AF$108</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="314">
   <si>
     <t>orderID</t>
   </si>
@@ -962,6 +962,9 @@
   </si>
   <si>
     <t>employeesLastName</t>
+  </si>
+  <si>
+    <t>productUnitPrice</t>
   </si>
 </sst>
 </file>
@@ -1811,9 +1814,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE108"/>
+  <dimension ref="A1:AF108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W108"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1839,20 +1844,21 @@
     <col min="20" max="20" width="15.42578125" style="1" customWidth="1"/>
     <col min="21" max="21" width="20.140625" style="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="16.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="15.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="29" style="1" customWidth="1"/>
-    <col min="30" max="30" width="29.28515625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="33.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="24.28515625" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="23" width="17.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="29" style="1" customWidth="1"/>
+    <col min="31" max="31" width="29.28515625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="33.140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="24.28515625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1920,34 +1926,37 @@
         <v>18</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10272</v>
       </c>
@@ -2018,31 +2027,34 @@
         <v>34.799999999999997</v>
       </c>
       <c r="X2" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="Y2" s="1">
         <v>14</v>
       </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
       <c r="Z2" s="1">
         <v>0</v>
       </c>
       <c r="AA2" s="1">
         <v>0</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10249</v>
       </c>
@@ -2113,31 +2125,34 @@
         <v>23.25</v>
       </c>
       <c r="X3" s="1">
+        <v>23.25</v>
+      </c>
+      <c r="Y3" s="1">
         <v>35</v>
       </c>
-      <c r="Y3" s="1">
-        <v>0</v>
-      </c>
       <c r="Z3" s="1">
         <v>0</v>
       </c>
       <c r="AA3" s="1">
         <v>0</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>10249</v>
       </c>
@@ -2208,31 +2223,34 @@
         <v>53</v>
       </c>
       <c r="X4" s="1">
+        <v>53</v>
+      </c>
+      <c r="Y4" s="1">
         <v>20</v>
       </c>
-      <c r="Y4" s="1">
-        <v>0</v>
-      </c>
       <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
         <v>10</v>
       </c>
-      <c r="AA4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10250</v>
       </c>
@@ -2303,31 +2321,34 @@
         <v>53</v>
       </c>
       <c r="X5" s="1">
+        <v>53</v>
+      </c>
+      <c r="Y5" s="1">
         <v>20</v>
       </c>
-      <c r="Y5" s="1">
-        <v>0</v>
-      </c>
       <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
         <v>10</v>
       </c>
-      <c r="AA5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10255</v>
       </c>
@@ -2398,31 +2419,34 @@
         <v>55</v>
       </c>
       <c r="X6" s="1">
+        <v>55</v>
+      </c>
+      <c r="Y6" s="1">
         <v>79</v>
       </c>
-      <c r="Y6" s="1">
-        <v>0</v>
-      </c>
       <c r="Z6" s="1">
         <v>0</v>
       </c>
       <c r="AA6" s="1">
         <v>0</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10250</v>
       </c>
@@ -2493,31 +2517,34 @@
         <v>9.65</v>
       </c>
       <c r="X7" s="1">
+        <v>9.65</v>
+      </c>
+      <c r="Y7" s="1">
         <v>85</v>
       </c>
-      <c r="Y7" s="1">
-        <v>0</v>
-      </c>
       <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
         <v>10</v>
       </c>
-      <c r="AA7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AE7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10255</v>
       </c>
@@ -2588,31 +2615,34 @@
         <v>17.45</v>
       </c>
       <c r="X8" s="1">
+        <v>17.45</v>
+      </c>
+      <c r="Y8" s="1">
         <v>29</v>
       </c>
-      <c r="Y8" s="1">
-        <v>0</v>
-      </c>
       <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
         <v>10</v>
       </c>
-      <c r="AA8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>304</v>
       </c>
       <c r="AE8" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF8" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>10253</v>
       </c>
@@ -2683,31 +2713,34 @@
         <v>12.5</v>
       </c>
       <c r="X9" s="1">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
         <v>70</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="AA9" s="1">
         <v>20</v>
       </c>
-      <c r="AA9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC9" s="1" t="s">
+      <c r="AD9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AE9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AF9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10272</v>
       </c>
@@ -2778,31 +2811,34 @@
         <v>12.5</v>
       </c>
       <c r="X10" s="1">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
         <v>70</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AA10" s="1">
         <v>20</v>
       </c>
-      <c r="AA10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC10" s="1" t="s">
+      <c r="AD10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AE10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE10" s="1" t="s">
+      <c r="AF10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10253</v>
       </c>
@@ -2873,31 +2909,34 @@
         <v>20</v>
       </c>
       <c r="X11" s="1">
+        <v>20</v>
+      </c>
+      <c r="Y11" s="1">
         <v>10</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Z11" s="1">
         <v>60</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AA11" s="1">
         <v>15</v>
       </c>
-      <c r="AA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AD11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AE11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AF11" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10272</v>
       </c>
@@ -2968,31 +3007,34 @@
         <v>81</v>
       </c>
       <c r="X12" s="1">
+        <v>81</v>
+      </c>
+      <c r="Y12" s="1">
         <v>40</v>
       </c>
-      <c r="Y12" s="1">
-        <v>0</v>
-      </c>
       <c r="Z12" s="1">
         <v>0</v>
       </c>
       <c r="AA12" s="1">
         <v>0</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD12" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE12" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF12" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10255</v>
       </c>
@@ -3063,31 +3105,34 @@
         <v>19</v>
       </c>
       <c r="X13" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y13" s="1">
         <v>112</v>
       </c>
-      <c r="Y13" s="1">
-        <v>0</v>
-      </c>
       <c r="Z13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
         <v>20</v>
       </c>
-      <c r="AA13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="1" t="s">
+      <c r="AB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC13" s="1" t="s">
+      <c r="AD13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD13" s="1" t="s">
+      <c r="AE13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AE13" s="1" t="s">
+      <c r="AF13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10273</v>
       </c>
@@ -3161,7 +3206,7 @@
         <v>31</v>
       </c>
       <c r="Y14" s="1">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="Z14" s="1">
         <v>0</v>
@@ -3169,20 +3214,23 @@
       <c r="AA14" s="1">
         <v>0</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AB14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AE14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AE14" s="1" t="s">
+      <c r="AF14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>10273</v>
       </c>
@@ -3253,31 +3301,34 @@
         <v>12.5</v>
       </c>
       <c r="X15" s="1">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="Y15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1">
         <v>70</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AA15" s="1">
         <v>20</v>
       </c>
-      <c r="AA15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="1" t="s">
+      <c r="AB15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC15" s="1" t="s">
+      <c r="AD15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD15" s="1" t="s">
+      <c r="AE15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE15" s="1" t="s">
+      <c r="AF15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>10273</v>
       </c>
@@ -3348,31 +3399,34 @@
         <v>2.5</v>
       </c>
       <c r="X16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Y16" s="1">
         <v>112</v>
       </c>
-      <c r="Y16" s="1">
-        <v>0</v>
-      </c>
       <c r="Z16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
         <v>20</v>
       </c>
-      <c r="AA16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="1" t="s">
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC16" s="1" t="s">
+      <c r="AD16" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD16" s="1" t="s">
+      <c r="AE16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE16" s="1" t="s">
+      <c r="AF16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>10273</v>
       </c>
@@ -3443,31 +3497,34 @@
         <v>18.399999999999999</v>
       </c>
       <c r="X17" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Y17" s="1">
         <v>123</v>
       </c>
-      <c r="Y17" s="1">
-        <v>0</v>
-      </c>
       <c r="Z17" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC17" s="1" t="s">
+      <c r="AD17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AD17" s="1" t="s">
+      <c r="AE17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AE17" s="1" t="s">
+      <c r="AF17" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10273</v>
       </c>
@@ -3538,31 +3595,34 @@
         <v>18</v>
       </c>
       <c r="X18" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y18" s="1">
         <v>57</v>
       </c>
-      <c r="Y18" s="1">
-        <v>0</v>
-      </c>
       <c r="Z18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1">
         <v>20</v>
       </c>
-      <c r="AA18" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AD18" s="1" t="s">
+      <c r="AE18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AE18" s="1" t="s">
+      <c r="AF18" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10276</v>
       </c>
@@ -3636,7 +3696,7 @@
         <v>31</v>
       </c>
       <c r="Y19" s="1">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
@@ -3644,20 +3704,23 @@
       <c r="AA19" s="1">
         <v>0</v>
       </c>
-      <c r="AB19" s="1" t="s">
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC19" s="1" t="s">
+      <c r="AD19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AD19" s="1" t="s">
+      <c r="AE19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AE19" s="1" t="s">
+      <c r="AF19" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10276</v>
       </c>
@@ -3728,31 +3791,34 @@
         <v>6</v>
       </c>
       <c r="X20" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="1">
         <v>24</v>
       </c>
-      <c r="Y20" s="1">
-        <v>0</v>
-      </c>
       <c r="Z20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1">
         <v>5</v>
       </c>
-      <c r="AA20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AE20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE20" s="1" t="s">
+      <c r="AF20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>10293</v>
       </c>
@@ -3823,31 +3889,34 @@
         <v>62.5</v>
       </c>
       <c r="X21" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="Y21" s="1">
         <v>42</v>
       </c>
-      <c r="Y21" s="1">
-        <v>0</v>
-      </c>
       <c r="Z21" s="1">
         <v>0</v>
       </c>
       <c r="AA21" s="1">
         <v>0</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="AD21" s="1" t="s">
         <v>304</v>
       </c>
       <c r="AE21" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF21" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10298</v>
       </c>
@@ -3918,31 +3987,34 @@
         <v>19</v>
       </c>
       <c r="X22" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y22" s="1">
         <v>17</v>
       </c>
-      <c r="Y22" s="1">
+      <c r="Z22" s="1">
         <v>40</v>
       </c>
-      <c r="Z22" s="1">
+      <c r="AA22" s="1">
         <v>25</v>
       </c>
-      <c r="AA22" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AD22" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AD22" s="1" t="s">
+      <c r="AE22" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AE22" s="1" t="s">
+      <c r="AF22" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10298</v>
       </c>
@@ -4013,31 +4085,34 @@
         <v>19</v>
       </c>
       <c r="X23" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y23" s="1">
         <v>112</v>
       </c>
-      <c r="Y23" s="1">
-        <v>0</v>
-      </c>
       <c r="Z23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
         <v>20</v>
       </c>
-      <c r="AA23" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="1" t="s">
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC23" s="1" t="s">
+      <c r="AD23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD23" s="1" t="s">
+      <c r="AE23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AE23" s="1" t="s">
+      <c r="AF23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10304</v>
       </c>
@@ -4108,31 +4183,34 @@
         <v>20</v>
       </c>
       <c r="X24" s="1">
+        <v>20</v>
+      </c>
+      <c r="Y24" s="1">
         <v>10</v>
       </c>
-      <c r="Y24" s="1">
+      <c r="Z24" s="1">
         <v>60</v>
       </c>
-      <c r="Z24" s="1">
+      <c r="AA24" s="1">
         <v>15</v>
       </c>
-      <c r="AA24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="1" t="s">
+      <c r="AB24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC24" s="1" t="s">
+      <c r="AD24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AD24" s="1" t="s">
+      <c r="AE24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AE24" s="1" t="s">
+      <c r="AF24" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>10304</v>
       </c>
@@ -4203,31 +4281,34 @@
         <v>55</v>
       </c>
       <c r="X25" s="1">
+        <v>55</v>
+      </c>
+      <c r="Y25" s="1">
         <v>79</v>
       </c>
-      <c r="Y25" s="1">
-        <v>0</v>
-      </c>
       <c r="Z25" s="1">
         <v>0</v>
       </c>
       <c r="AA25" s="1">
         <v>0</v>
       </c>
-      <c r="AB25" s="1" t="s">
+      <c r="AB25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC25" s="1" t="s">
+      <c r="AD25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD25" s="1" t="s">
+      <c r="AE25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AE25" s="1" t="s">
+      <c r="AF25" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>10304</v>
       </c>
@@ -4298,31 +4379,34 @@
         <v>21.5</v>
       </c>
       <c r="X26" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="Y26" s="1">
         <v>26</v>
       </c>
-      <c r="Y26" s="1">
-        <v>0</v>
-      </c>
       <c r="Z26" s="1">
         <v>0</v>
       </c>
       <c r="AA26" s="1">
         <v>0</v>
       </c>
-      <c r="AB26" s="1" t="s">
+      <c r="AB26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC26" s="1" t="s">
+      <c r="AD26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD26" s="1" t="s">
+      <c r="AE26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE26" s="1" t="s">
+      <c r="AF26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>10321</v>
       </c>
@@ -4393,31 +4477,34 @@
         <v>18</v>
       </c>
       <c r="X27" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y27" s="1">
         <v>20</v>
       </c>
-      <c r="Y27" s="1">
-        <v>0</v>
-      </c>
       <c r="Z27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
         <v>15</v>
       </c>
-      <c r="AA27" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="1" t="s">
+      <c r="AB27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC27" s="1" t="s">
+      <c r="AD27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AD27" s="1" t="s">
+      <c r="AE27" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AE27" s="1" t="s">
+      <c r="AF27" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>10344</v>
       </c>
@@ -4488,31 +4575,34 @@
         <v>22</v>
       </c>
       <c r="X28" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y28" s="1">
         <v>53</v>
       </c>
-      <c r="Y28" s="1">
-        <v>0</v>
-      </c>
       <c r="Z28" s="1">
         <v>0</v>
       </c>
       <c r="AA28" s="1">
         <v>0</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC28" s="1" t="s">
+      <c r="AD28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AD28" s="1" t="s">
+      <c r="AE28" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AE28" s="1" t="s">
+      <c r="AF28" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>10344</v>
       </c>
@@ -4583,31 +4673,34 @@
         <v>40</v>
       </c>
       <c r="X29" s="1">
+        <v>40</v>
+      </c>
+      <c r="Y29" s="1">
         <v>6</v>
       </c>
-      <c r="Y29" s="1">
-        <v>0</v>
-      </c>
       <c r="Z29" s="1">
         <v>0</v>
       </c>
       <c r="AA29" s="1">
         <v>0</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AB29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC29" s="1" t="s">
+      <c r="AD29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AD29" s="1" t="s">
+      <c r="AE29" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AE29" s="1" t="s">
+      <c r="AF29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>10346</v>
       </c>
@@ -4678,31 +4771,34 @@
         <v>38</v>
       </c>
       <c r="X30" s="1">
+        <v>38</v>
+      </c>
+      <c r="Y30" s="1">
         <v>21</v>
       </c>
-      <c r="Y30" s="1">
+      <c r="Z30" s="1">
         <v>10</v>
       </c>
-      <c r="Z30" s="1">
-        <v>30</v>
-      </c>
       <c r="AA30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC30" s="1" t="s">
+      <c r="AD30" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AD30" s="1" t="s">
+      <c r="AE30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AE30" s="1" t="s">
+      <c r="AF30" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>10372</v>
       </c>
@@ -4773,31 +4869,34 @@
         <v>81</v>
       </c>
       <c r="X31" s="1">
+        <v>81</v>
+      </c>
+      <c r="Y31" s="1">
         <v>40</v>
       </c>
-      <c r="Y31" s="1">
-        <v>0</v>
-      </c>
       <c r="Z31" s="1">
         <v>0</v>
       </c>
       <c r="AA31" s="1">
         <v>0</v>
       </c>
-      <c r="AB31" s="1" t="s">
+      <c r="AB31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC31" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD31" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE31" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF31" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>10372</v>
       </c>
@@ -4868,31 +4967,34 @@
         <v>263.5</v>
       </c>
       <c r="X32" s="1">
+        <v>263.5</v>
+      </c>
+      <c r="Y32" s="1">
         <v>17</v>
       </c>
-      <c r="Y32" s="1">
-        <v>0</v>
-      </c>
       <c r="Z32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="1">
         <v>15</v>
       </c>
-      <c r="AA32" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="1" t="s">
+      <c r="AB32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC32" s="1" t="s">
+      <c r="AD32" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AD32" s="1" t="s">
+      <c r="AE32" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="AE32" s="1" t="s">
+      <c r="AF32" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>10372</v>
       </c>
@@ -4963,31 +5065,34 @@
         <v>34</v>
       </c>
       <c r="X33" s="1">
+        <v>34</v>
+      </c>
+      <c r="Y33" s="1">
         <v>19</v>
       </c>
-      <c r="Y33" s="1">
-        <v>0</v>
-      </c>
       <c r="Z33" s="1">
         <v>0</v>
       </c>
       <c r="AA33" s="1">
         <v>0</v>
       </c>
-      <c r="AB33" s="1" t="s">
+      <c r="AB33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC33" s="1" t="s">
+      <c r="AD33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD33" s="1" t="s">
+      <c r="AE33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AE33" s="1" t="s">
+      <c r="AF33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>10372</v>
       </c>
@@ -5058,31 +5163,34 @@
         <v>34.799999999999997</v>
       </c>
       <c r="X34" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="Y34" s="1">
         <v>14</v>
       </c>
-      <c r="Y34" s="1">
-        <v>0</v>
-      </c>
       <c r="Z34" s="1">
         <v>0</v>
       </c>
       <c r="AA34" s="1">
         <v>0</v>
       </c>
-      <c r="AB34" s="1" t="s">
+      <c r="AB34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC34" s="1" t="s">
+      <c r="AD34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD34" s="1" t="s">
+      <c r="AE34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE34" s="1" t="s">
+      <c r="AF34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>10373</v>
       </c>
@@ -5153,31 +5261,34 @@
         <v>13.25</v>
       </c>
       <c r="X35" s="1">
+        <v>13.25</v>
+      </c>
+      <c r="Y35" s="1">
         <v>62</v>
       </c>
-      <c r="Y35" s="1">
-        <v>0</v>
-      </c>
       <c r="Z35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="1">
         <v>20</v>
       </c>
-      <c r="AA35" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="1" t="s">
+      <c r="AB35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC35" s="1" t="s">
+      <c r="AD35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AD35" s="1" t="s">
+      <c r="AE35" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="AE35" s="1" t="s">
+      <c r="AF35" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>10373</v>
       </c>
@@ -5248,31 +5359,34 @@
         <v>21.5</v>
       </c>
       <c r="X36" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="Y36" s="1">
         <v>26</v>
       </c>
-      <c r="Y36" s="1">
-        <v>0</v>
-      </c>
       <c r="Z36" s="1">
         <v>0</v>
       </c>
       <c r="AA36" s="1">
         <v>0</v>
       </c>
-      <c r="AB36" s="1" t="s">
+      <c r="AB36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC36" s="1" t="s">
+      <c r="AD36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD36" s="1" t="s">
+      <c r="AE36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE36" s="1" t="s">
+      <c r="AF36" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>10375</v>
       </c>
@@ -5343,31 +5457,34 @@
         <v>23.25</v>
       </c>
       <c r="X37" s="1">
+        <v>23.25</v>
+      </c>
+      <c r="Y37" s="1">
         <v>35</v>
       </c>
-      <c r="Y37" s="1">
-        <v>0</v>
-      </c>
       <c r="Z37" s="1">
         <v>0</v>
       </c>
       <c r="AA37" s="1">
         <v>0</v>
       </c>
-      <c r="AB37" s="1" t="s">
+      <c r="AB37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC37" s="1" t="s">
+      <c r="AD37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD37" s="1" t="s">
+      <c r="AE37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE37" s="1" t="s">
+      <c r="AF37" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>10377</v>
       </c>
@@ -5438,31 +5555,34 @@
         <v>45.6</v>
       </c>
       <c r="X38" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="Y38" s="1">
         <v>26</v>
       </c>
-      <c r="Y38" s="1">
-        <v>0</v>
-      </c>
       <c r="Z38" s="1">
         <v>0</v>
       </c>
       <c r="AA38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="1">
         <v>1</v>
       </c>
-      <c r="AB38" s="1" t="s">
+      <c r="AC38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC38" s="1" t="s">
+      <c r="AD38" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD38" s="1" t="s">
+      <c r="AE38" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE38" s="1" t="s">
+      <c r="AF38" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>10377</v>
       </c>
@@ -5533,31 +5653,34 @@
         <v>18</v>
       </c>
       <c r="X39" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y39" s="1">
         <v>69</v>
       </c>
-      <c r="Y39" s="1">
-        <v>0</v>
-      </c>
       <c r="Z39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="1">
         <v>5</v>
       </c>
-      <c r="AA39" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="1" t="s">
+      <c r="AB39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC39" s="1" t="s">
+      <c r="AD39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AD39" s="1" t="s">
+      <c r="AE39" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="AE39" s="1" t="s">
+      <c r="AF39" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>10380</v>
       </c>
@@ -5628,31 +5751,34 @@
         <v>25.89</v>
       </c>
       <c r="X40" s="1">
+        <v>25.89</v>
+      </c>
+      <c r="Y40" s="1">
         <v>10</v>
       </c>
-      <c r="Y40" s="1">
-        <v>0</v>
-      </c>
       <c r="Z40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="1">
         <v>15</v>
       </c>
-      <c r="AA40" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="1" t="s">
+      <c r="AB40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC40" s="1" t="s">
+      <c r="AD40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD40" s="1" t="s">
+      <c r="AE40" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AE40" s="1" t="s">
+      <c r="AF40" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>10380</v>
       </c>
@@ -5723,7 +5849,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="X41" s="1">
-        <v>0</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="Y41" s="1">
         <v>0</v>
@@ -5732,22 +5858,25 @@
         <v>0</v>
       </c>
       <c r="AA41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="1">
         <v>1</v>
       </c>
-      <c r="AB41" s="1" t="s">
+      <c r="AC41" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AC41" s="1" t="s">
+      <c r="AD41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD41" s="1" t="s">
+      <c r="AE41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE41" s="1" t="s">
+      <c r="AF41" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>10395</v>
       </c>
@@ -5818,31 +5947,34 @@
         <v>36</v>
       </c>
       <c r="X42" s="1">
+        <v>36</v>
+      </c>
+      <c r="Y42" s="1">
         <v>26</v>
       </c>
-      <c r="Y42" s="1">
-        <v>0</v>
-      </c>
       <c r="Z42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="1">
         <v>15</v>
       </c>
-      <c r="AA42" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB42" s="1" t="s">
+      <c r="AB42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC42" s="1" t="s">
+      <c r="AD42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD42" s="1" t="s">
+      <c r="AE42" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE42" s="1" t="s">
+      <c r="AF42" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>10400</v>
       </c>
@@ -5913,31 +6045,34 @@
         <v>18</v>
       </c>
       <c r="X43" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y43" s="1">
         <v>20</v>
       </c>
-      <c r="Y43" s="1">
-        <v>0</v>
-      </c>
       <c r="Z43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="1">
         <v>15</v>
       </c>
-      <c r="AA43" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB43" s="1" t="s">
+      <c r="AB43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC43" s="1" t="s">
+      <c r="AD43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AD43" s="1" t="s">
+      <c r="AE43" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AE43" s="1" t="s">
+      <c r="AF43" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>10401</v>
       </c>
@@ -6008,31 +6143,34 @@
         <v>25.89</v>
       </c>
       <c r="X44" s="1">
+        <v>25.89</v>
+      </c>
+      <c r="Y44" s="1">
         <v>10</v>
       </c>
-      <c r="Y44" s="1">
-        <v>0</v>
-      </c>
       <c r="Z44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="1">
         <v>15</v>
       </c>
-      <c r="AA44" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="1" t="s">
+      <c r="AB44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC44" s="1" t="s">
+      <c r="AD44" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD44" s="1" t="s">
+      <c r="AE44" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AE44" s="1" t="s">
+      <c r="AF44" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>10401</v>
       </c>
@@ -6103,31 +6241,34 @@
         <v>38</v>
       </c>
       <c r="X45" s="1">
+        <v>38</v>
+      </c>
+      <c r="Y45" s="1">
         <v>21</v>
       </c>
-      <c r="Y45" s="1">
+      <c r="Z45" s="1">
         <v>10</v>
       </c>
-      <c r="Z45" s="1">
-        <v>30</v>
-      </c>
       <c r="AA45" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC45" s="1" t="s">
+      <c r="AD45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AD45" s="1" t="s">
+      <c r="AE45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AE45" s="1" t="s">
+      <c r="AF45" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>10401</v>
       </c>
@@ -6198,31 +6339,34 @@
         <v>21.05</v>
       </c>
       <c r="X46" s="1">
+        <v>21.05</v>
+      </c>
+      <c r="Y46" s="1">
         <v>76</v>
       </c>
-      <c r="Y46" s="1">
-        <v>0</v>
-      </c>
       <c r="Z46" s="1">
         <v>0</v>
       </c>
       <c r="AA46" s="1">
         <v>0</v>
       </c>
-      <c r="AB46" s="1" t="s">
+      <c r="AB46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC46" s="1" t="s">
+      <c r="AD46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AD46" s="1" t="s">
+      <c r="AE46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AE46" s="1" t="s">
+      <c r="AF46" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>10401</v>
       </c>
@@ -6293,31 +6437,34 @@
         <v>21.5</v>
       </c>
       <c r="X47" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="Y47" s="1">
         <v>26</v>
       </c>
-      <c r="Y47" s="1">
-        <v>0</v>
-      </c>
       <c r="Z47" s="1">
         <v>0</v>
       </c>
       <c r="AA47" s="1">
         <v>0</v>
       </c>
-      <c r="AB47" s="1" t="s">
+      <c r="AB47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC47" s="1" t="s">
+      <c r="AD47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD47" s="1" t="s">
+      <c r="AE47" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE47" s="1" t="s">
+      <c r="AF47" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>10406</v>
       </c>
@@ -6388,31 +6535,34 @@
         <v>18</v>
       </c>
       <c r="X48" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y48" s="1">
         <v>39</v>
       </c>
-      <c r="Y48" s="1">
-        <v>0</v>
-      </c>
       <c r="Z48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="1">
         <v>10</v>
       </c>
-      <c r="AA48" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB48" s="1" t="s">
+      <c r="AB48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC48" s="1" t="s">
+      <c r="AD48" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AD48" s="1" t="s">
+      <c r="AE48" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="AE48" s="1" t="s">
+      <c r="AF48" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>10406</v>
       </c>
@@ -6483,31 +6633,34 @@
         <v>10</v>
       </c>
       <c r="X49" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y49" s="1">
         <v>3</v>
       </c>
-      <c r="Y49" s="1">
+      <c r="Z49" s="1">
         <v>40</v>
       </c>
-      <c r="Z49" s="1">
+      <c r="AA49" s="1">
         <v>5</v>
       </c>
-      <c r="AA49" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB49" s="1" t="s">
+      <c r="AB49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC49" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD49" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE49" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF49" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>10406</v>
       </c>
@@ -6578,31 +6731,34 @@
         <v>45.6</v>
       </c>
       <c r="X50" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="Y50" s="1">
         <v>26</v>
       </c>
-      <c r="Y50" s="1">
-        <v>0</v>
-      </c>
       <c r="Z50" s="1">
         <v>0</v>
       </c>
       <c r="AA50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="1">
         <v>1</v>
       </c>
-      <c r="AB50" s="1" t="s">
+      <c r="AC50" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC50" s="1" t="s">
+      <c r="AD50" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD50" s="1" t="s">
+      <c r="AE50" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE50" s="1" t="s">
+      <c r="AF50" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>10406</v>
       </c>
@@ -6673,31 +6829,34 @@
         <v>19</v>
       </c>
       <c r="X51" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y51" s="1">
         <v>112</v>
       </c>
-      <c r="Y51" s="1">
-        <v>0</v>
-      </c>
       <c r="Z51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="1">
         <v>20</v>
       </c>
-      <c r="AA51" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB51" s="1" t="s">
+      <c r="AB51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC51" s="1" t="s">
+      <c r="AD51" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD51" s="1" t="s">
+      <c r="AE51" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AE51" s="1" t="s">
+      <c r="AF51" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>10406</v>
       </c>
@@ -6768,31 +6927,34 @@
         <v>18.399999999999999</v>
       </c>
       <c r="X52" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Y52" s="1">
         <v>123</v>
       </c>
-      <c r="Y52" s="1">
-        <v>0</v>
-      </c>
       <c r="Z52" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC52" s="1" t="s">
+      <c r="AD52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AD52" s="1" t="s">
+      <c r="AE52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AE52" s="1" t="s">
+      <c r="AF52" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>10410</v>
       </c>
@@ -6863,31 +7025,34 @@
         <v>2.5</v>
       </c>
       <c r="X53" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Y53" s="1">
         <v>112</v>
       </c>
-      <c r="Y53" s="1">
-        <v>0</v>
-      </c>
       <c r="Z53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="1">
         <v>20</v>
       </c>
-      <c r="AA53" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB53" s="1" t="s">
+      <c r="AB53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC53" s="1" t="s">
+      <c r="AD53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD53" s="1" t="s">
+      <c r="AE53" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE53" s="1" t="s">
+      <c r="AF53" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>10411</v>
       </c>
@@ -6958,31 +7123,34 @@
         <v>19.45</v>
       </c>
       <c r="X54" s="1">
+        <v>19.45</v>
+      </c>
+      <c r="Y54" s="1">
         <v>27</v>
       </c>
-      <c r="Y54" s="1">
-        <v>0</v>
-      </c>
       <c r="Z54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="1">
         <v>15</v>
       </c>
-      <c r="AA54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB54" s="1" t="s">
+      <c r="AB54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC54" s="1" t="s">
+      <c r="AD54" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AD54" s="1" t="s">
+      <c r="AE54" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AE54" s="1" t="s">
+      <c r="AF54" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>10411</v>
       </c>
@@ -7053,31 +7221,34 @@
         <v>55</v>
       </c>
       <c r="X55" s="1">
+        <v>55</v>
+      </c>
+      <c r="Y55" s="1">
         <v>79</v>
       </c>
-      <c r="Y55" s="1">
-        <v>0</v>
-      </c>
       <c r="Z55" s="1">
         <v>0</v>
       </c>
       <c r="AA55" s="1">
         <v>0</v>
       </c>
-      <c r="AB55" s="1" t="s">
+      <c r="AB55" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC55" s="1" t="s">
+      <c r="AD55" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD55" s="1" t="s">
+      <c r="AE55" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AE55" s="1" t="s">
+      <c r="AF55" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>10435</v>
       </c>
@@ -7148,31 +7319,34 @@
         <v>19</v>
       </c>
       <c r="X56" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y56" s="1">
         <v>17</v>
       </c>
-      <c r="Y56" s="1">
+      <c r="Z56" s="1">
         <v>40</v>
       </c>
-      <c r="Z56" s="1">
+      <c r="AA56" s="1">
         <v>25</v>
       </c>
-      <c r="AA56" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB56" s="1" t="s">
+      <c r="AB56" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC56" s="1" t="s">
+      <c r="AD56" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AD56" s="1" t="s">
+      <c r="AE56" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AE56" s="1" t="s">
+      <c r="AF56" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>10435</v>
       </c>
@@ -7243,31 +7417,34 @@
         <v>34.799999999999997</v>
       </c>
       <c r="X57" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="Y57" s="1">
         <v>14</v>
       </c>
-      <c r="Y57" s="1">
-        <v>0</v>
-      </c>
       <c r="Z57" s="1">
         <v>0</v>
       </c>
       <c r="AA57" s="1">
         <v>0</v>
       </c>
-      <c r="AB57" s="1" t="s">
+      <c r="AB57" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC57" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC57" s="1" t="s">
+      <c r="AD57" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD57" s="1" t="s">
+      <c r="AE57" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE57" s="1" t="s">
+      <c r="AF57" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>10438</v>
       </c>
@@ -7338,31 +7515,34 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="X58" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Y58" s="1">
         <v>25</v>
       </c>
-      <c r="Y58" s="1">
-        <v>0</v>
-      </c>
       <c r="Z58" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA58" s="1">
         <v>5</v>
       </c>
-      <c r="AA58" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB58" s="1" t="s">
+      <c r="AB58" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC58" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD58" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE58" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF58" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>10438</v>
       </c>
@@ -7433,31 +7613,34 @@
         <v>14</v>
       </c>
       <c r="X59" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y59" s="1">
         <v>111</v>
       </c>
-      <c r="Y59" s="1">
-        <v>0</v>
-      </c>
       <c r="Z59" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA59" s="1">
         <v>15</v>
       </c>
-      <c r="AA59" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB59" s="1" t="s">
+      <c r="AB59" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC59" s="1" t="s">
+      <c r="AD59" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AD59" s="1" t="s">
+      <c r="AE59" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AE59" s="1" t="s">
+      <c r="AF59" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>10438</v>
       </c>
@@ -7528,31 +7711,34 @@
         <v>19.5</v>
       </c>
       <c r="X60" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="Y60" s="1">
         <v>36</v>
       </c>
-      <c r="Y60" s="1">
-        <v>0</v>
-      </c>
       <c r="Z60" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA60" s="1">
         <v>20</v>
       </c>
-      <c r="AA60" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="1" t="s">
+      <c r="AB60" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC60" s="1" t="s">
+      <c r="AD60" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AD60" s="1" t="s">
+      <c r="AE60" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AE60" s="1" t="s">
+      <c r="AF60" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>10441</v>
       </c>
@@ -7623,31 +7809,34 @@
         <v>43.9</v>
       </c>
       <c r="X61" s="1">
+        <v>43.9</v>
+      </c>
+      <c r="Y61" s="1">
         <v>49</v>
       </c>
-      <c r="Y61" s="1">
-        <v>0</v>
-      </c>
       <c r="Z61" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA61" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB61" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC61" s="1" t="s">
+      <c r="AD61" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="AD61" s="1" t="s">
+      <c r="AE61" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AE61" s="1" t="s">
+      <c r="AF61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>10469</v>
       </c>
@@ -7718,31 +7907,34 @@
         <v>19</v>
       </c>
       <c r="X62" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y62" s="1">
         <v>17</v>
       </c>
-      <c r="Y62" s="1">
+      <c r="Z62" s="1">
         <v>40</v>
       </c>
-      <c r="Z62" s="1">
+      <c r="AA62" s="1">
         <v>25</v>
       </c>
-      <c r="AA62" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="1" t="s">
+      <c r="AB62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC62" s="1" t="s">
+      <c r="AD62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AD62" s="1" t="s">
+      <c r="AE62" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AE62" s="1" t="s">
+      <c r="AF62" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>10469</v>
       </c>
@@ -7813,31 +8005,34 @@
         <v>17.45</v>
       </c>
       <c r="X63" s="1">
+        <v>17.45</v>
+      </c>
+      <c r="Y63" s="1">
         <v>29</v>
       </c>
-      <c r="Y63" s="1">
-        <v>0</v>
-      </c>
       <c r="Z63" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA63" s="1">
         <v>10</v>
       </c>
-      <c r="AA63" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB63" s="1" t="s">
+      <c r="AB63" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC63" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="AD63" s="1" t="s">
         <v>304</v>
       </c>
       <c r="AE63" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF63" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>10469</v>
       </c>
@@ -7908,31 +8103,34 @@
         <v>19.45</v>
       </c>
       <c r="X64" s="1">
+        <v>19.45</v>
+      </c>
+      <c r="Y64" s="1">
         <v>27</v>
       </c>
-      <c r="Y64" s="1">
-        <v>0</v>
-      </c>
       <c r="Z64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="1">
         <v>15</v>
       </c>
-      <c r="AA64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB64" s="1" t="s">
+      <c r="AB64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC64" s="1" t="s">
+      <c r="AD64" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AD64" s="1" t="s">
+      <c r="AE64" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AE64" s="1" t="s">
+      <c r="AF64" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>10471</v>
       </c>
@@ -8003,31 +8201,34 @@
         <v>30</v>
       </c>
       <c r="X65" s="1">
+        <v>30</v>
+      </c>
+      <c r="Y65" s="1">
         <v>15</v>
       </c>
-      <c r="Y65" s="1">
-        <v>0</v>
-      </c>
       <c r="Z65" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA65" s="1">
         <v>10</v>
       </c>
-      <c r="AA65" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB65" s="1" t="s">
+      <c r="AB65" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC65" s="1" t="s">
+      <c r="AD65" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AD65" s="1" t="s">
+      <c r="AE65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="AE65" s="1" t="s">
+      <c r="AF65" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>10471</v>
       </c>
@@ -8098,31 +8299,34 @@
         <v>38</v>
       </c>
       <c r="X66" s="1">
+        <v>38</v>
+      </c>
+      <c r="Y66" s="1">
         <v>21</v>
       </c>
-      <c r="Y66" s="1">
+      <c r="Z66" s="1">
         <v>10</v>
       </c>
-      <c r="Z66" s="1">
-        <v>30</v>
-      </c>
       <c r="AA66" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB66" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC66" s="1" t="s">
+      <c r="AD66" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AD66" s="1" t="s">
+      <c r="AE66" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AE66" s="1" t="s">
+      <c r="AF66" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>10472</v>
       </c>
@@ -8193,31 +8397,34 @@
         <v>4.5</v>
       </c>
       <c r="X67" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Y67" s="1">
         <v>20</v>
       </c>
-      <c r="Y67" s="1">
-        <v>0</v>
-      </c>
       <c r="Z67" s="1">
         <v>0</v>
       </c>
       <c r="AA67" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="1">
         <v>1</v>
       </c>
-      <c r="AB67" s="1" t="s">
+      <c r="AC67" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC67" s="1" t="s">
+      <c r="AD67" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AD67" s="1" t="s">
+      <c r="AE67" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="AE67" s="1" t="s">
+      <c r="AF67" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>10472</v>
       </c>
@@ -8288,31 +8495,34 @@
         <v>53</v>
       </c>
       <c r="X68" s="1">
+        <v>53</v>
+      </c>
+      <c r="Y68" s="1">
         <v>20</v>
       </c>
-      <c r="Y68" s="1">
-        <v>0</v>
-      </c>
       <c r="Z68" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="1">
         <v>10</v>
       </c>
-      <c r="AA68" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB68" s="1" t="s">
+      <c r="AB68" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC68" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC68" s="1" t="s">
+      <c r="AD68" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD68" s="1" t="s">
+      <c r="AE68" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE68" s="1" t="s">
+      <c r="AF68" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>10495</v>
       </c>
@@ -8383,31 +8593,34 @@
         <v>9</v>
       </c>
       <c r="X69" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y69" s="1">
         <v>61</v>
       </c>
-      <c r="Y69" s="1">
-        <v>0</v>
-      </c>
       <c r="Z69" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA69" s="1">
         <v>25</v>
       </c>
-      <c r="AA69" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB69" s="1" t="s">
+      <c r="AB69" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC69" s="1" t="s">
+      <c r="AD69" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="AD69" s="1" t="s">
+      <c r="AE69" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="AE69" s="1" t="s">
+      <c r="AF69" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>10495</v>
       </c>
@@ -8478,31 +8691,34 @@
         <v>9.65</v>
       </c>
       <c r="X70" s="1">
+        <v>9.65</v>
+      </c>
+      <c r="Y70" s="1">
         <v>85</v>
       </c>
-      <c r="Y70" s="1">
-        <v>0</v>
-      </c>
       <c r="Z70" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA70" s="1">
         <v>10</v>
       </c>
-      <c r="AA70" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB70" s="1" t="s">
+      <c r="AB70" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC70" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC70" s="1" t="s">
+      <c r="AD70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AD70" s="1" t="s">
+      <c r="AE70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AE70" s="1" t="s">
+      <c r="AF70" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>10495</v>
       </c>
@@ -8573,31 +8789,34 @@
         <v>13</v>
       </c>
       <c r="X71" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y71" s="1">
         <v>32</v>
       </c>
-      <c r="Y71" s="1">
-        <v>0</v>
-      </c>
       <c r="Z71" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA71" s="1">
         <v>15</v>
       </c>
-      <c r="AA71" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB71" s="1" t="s">
+      <c r="AB71" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC71" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC71" s="1" t="s">
+      <c r="AD71" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD71" s="1" t="s">
+      <c r="AE71" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE71" s="1" t="s">
+      <c r="AF71" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>10497</v>
       </c>
@@ -8668,31 +8887,34 @@
         <v>38</v>
       </c>
       <c r="X72" s="1">
+        <v>38</v>
+      </c>
+      <c r="Y72" s="1">
         <v>21</v>
       </c>
-      <c r="Y72" s="1">
+      <c r="Z72" s="1">
         <v>10</v>
       </c>
-      <c r="Z72" s="1">
-        <v>30</v>
-      </c>
       <c r="AA72" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC72" s="1" t="s">
+      <c r="AD72" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AD72" s="1" t="s">
+      <c r="AE72" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AE72" s="1" t="s">
+      <c r="AF72" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>10497</v>
       </c>
@@ -8763,31 +8985,34 @@
         <v>34.799999999999997</v>
       </c>
       <c r="X73" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="Y73" s="1">
         <v>14</v>
       </c>
-      <c r="Y73" s="1">
-        <v>0</v>
-      </c>
       <c r="Z73" s="1">
         <v>0</v>
       </c>
       <c r="AA73" s="1">
         <v>0</v>
       </c>
-      <c r="AB73" s="1" t="s">
+      <c r="AB73" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC73" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC73" s="1" t="s">
+      <c r="AD73" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD73" s="1" t="s">
+      <c r="AE73" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE73" s="1" t="s">
+      <c r="AF73" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>10497</v>
       </c>
@@ -8858,31 +9083,34 @@
         <v>13</v>
       </c>
       <c r="X74" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y74" s="1">
         <v>32</v>
       </c>
-      <c r="Y74" s="1">
-        <v>0</v>
-      </c>
       <c r="Z74" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA74" s="1">
         <v>15</v>
       </c>
-      <c r="AA74" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB74" s="1" t="s">
+      <c r="AB74" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC74" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC74" s="1" t="s">
+      <c r="AD74" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD74" s="1" t="s">
+      <c r="AE74" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE74" s="1" t="s">
+      <c r="AF74" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>10498</v>
       </c>
@@ -8953,31 +9181,34 @@
         <v>4.5</v>
       </c>
       <c r="X75" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Y75" s="1">
         <v>20</v>
       </c>
-      <c r="Y75" s="1">
-        <v>0</v>
-      </c>
       <c r="Z75" s="1">
         <v>0</v>
       </c>
       <c r="AA75" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB75" s="1">
         <v>1</v>
       </c>
-      <c r="AB75" s="1" t="s">
+      <c r="AC75" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC75" s="1" t="s">
+      <c r="AD75" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AD75" s="1" t="s">
+      <c r="AE75" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="AE75" s="1" t="s">
+      <c r="AF75" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>10498</v>
       </c>
@@ -9048,31 +9279,34 @@
         <v>18.399999999999999</v>
       </c>
       <c r="X76" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Y76" s="1">
         <v>123</v>
       </c>
-      <c r="Y76" s="1">
-        <v>0</v>
-      </c>
       <c r="Z76" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA76" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB76" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC76" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC76" s="1" t="s">
+      <c r="AD76" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AD76" s="1" t="s">
+      <c r="AE76" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AE76" s="1" t="s">
+      <c r="AF76" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>10503</v>
       </c>
@@ -9143,31 +9377,34 @@
         <v>23.25</v>
       </c>
       <c r="X77" s="1">
+        <v>23.25</v>
+      </c>
+      <c r="Y77" s="1">
         <v>35</v>
       </c>
-      <c r="Y77" s="1">
-        <v>0</v>
-      </c>
       <c r="Z77" s="1">
         <v>0</v>
       </c>
       <c r="AA77" s="1">
         <v>0</v>
       </c>
-      <c r="AB77" s="1" t="s">
+      <c r="AB77" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC77" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC77" s="1" t="s">
+      <c r="AD77" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD77" s="1" t="s">
+      <c r="AE77" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE77" s="1" t="s">
+      <c r="AF77" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>10503</v>
       </c>
@@ -9238,31 +9475,34 @@
         <v>21.05</v>
       </c>
       <c r="X78" s="1">
+        <v>21.05</v>
+      </c>
+      <c r="Y78" s="1">
         <v>76</v>
       </c>
-      <c r="Y78" s="1">
-        <v>0</v>
-      </c>
       <c r="Z78" s="1">
         <v>0</v>
       </c>
       <c r="AA78" s="1">
         <v>0</v>
       </c>
-      <c r="AB78" s="1" t="s">
+      <c r="AB78" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC78" s="1" t="s">
+      <c r="AD78" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AD78" s="1" t="s">
+      <c r="AE78" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AE78" s="1" t="s">
+      <c r="AF78" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>10504</v>
       </c>
@@ -9333,31 +9573,34 @@
         <v>19</v>
       </c>
       <c r="X79" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y79" s="1">
         <v>17</v>
       </c>
-      <c r="Y79" s="1">
+      <c r="Z79" s="1">
         <v>40</v>
       </c>
-      <c r="Z79" s="1">
+      <c r="AA79" s="1">
         <v>25</v>
       </c>
-      <c r="AA79" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB79" s="1" t="s">
+      <c r="AB79" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC79" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC79" s="1" t="s">
+      <c r="AD79" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AD79" s="1" t="s">
+      <c r="AE79" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AE79" s="1" t="s">
+      <c r="AF79" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>10504</v>
       </c>
@@ -9428,31 +9671,34 @@
         <v>10</v>
       </c>
       <c r="X80" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y80" s="1">
         <v>3</v>
       </c>
-      <c r="Y80" s="1">
+      <c r="Z80" s="1">
         <v>40</v>
       </c>
-      <c r="Z80" s="1">
+      <c r="AA80" s="1">
         <v>5</v>
       </c>
-      <c r="AA80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB80" s="1" t="s">
+      <c r="AB80" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC80" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC80" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD80" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE80" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF80" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>10504</v>
       </c>
@@ -9523,7 +9769,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="X81" s="1">
-        <v>0</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="Y81" s="1">
         <v>0</v>
@@ -9532,22 +9778,25 @@
         <v>0</v>
       </c>
       <c r="AA81" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB81" s="1">
         <v>1</v>
       </c>
-      <c r="AB81" s="1" t="s">
+      <c r="AC81" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AC81" s="1" t="s">
+      <c r="AD81" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD81" s="1" t="s">
+      <c r="AE81" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE81" s="1" t="s">
+      <c r="AF81" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>10504</v>
       </c>
@@ -9618,31 +9867,34 @@
         <v>28.5</v>
       </c>
       <c r="X82" s="1">
+        <v>28.5</v>
+      </c>
+      <c r="Y82" s="1">
         <v>113</v>
       </c>
-      <c r="Y82" s="1">
-        <v>0</v>
-      </c>
       <c r="Z82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="1">
         <v>25</v>
       </c>
-      <c r="AA82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB82" s="1" t="s">
+      <c r="AB82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC82" s="1" t="s">
+      <c r="AD82" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AD82" s="1" t="s">
+      <c r="AE82" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AE82" s="1" t="s">
+      <c r="AF82" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>10523</v>
       </c>
@@ -9713,7 +9965,7 @@
         <v>39</v>
       </c>
       <c r="X83" s="1">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="Y83" s="1">
         <v>0</v>
@@ -9722,22 +9974,25 @@
         <v>0</v>
       </c>
       <c r="AA83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="1">
         <v>1</v>
       </c>
-      <c r="AB83" s="1" t="s">
+      <c r="AC83" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="AC83" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="AD83" s="1" t="s">
         <v>304</v>
       </c>
       <c r="AE83" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF83" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>10529</v>
       </c>
@@ -9808,31 +10063,34 @@
         <v>24</v>
       </c>
       <c r="X84" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y84" s="1">
         <v>115</v>
       </c>
-      <c r="Y84" s="1">
-        <v>0</v>
-      </c>
       <c r="Z84" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA84" s="1">
         <v>20</v>
       </c>
-      <c r="AA84" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB84" s="1" t="s">
+      <c r="AB84" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC84" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AC84" s="1" t="s">
+      <c r="AD84" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AD84" s="1" t="s">
+      <c r="AE84" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AE84" s="1" t="s">
+      <c r="AF84" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>10529</v>
       </c>
@@ -9903,31 +10161,34 @@
         <v>12.5</v>
       </c>
       <c r="X85" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="Y85" s="1">
         <v>6</v>
       </c>
-      <c r="Y85" s="1">
+      <c r="Z85" s="1">
         <v>10</v>
       </c>
-      <c r="Z85" s="1">
+      <c r="AA85" s="1">
         <v>15</v>
       </c>
-      <c r="AA85" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB85" s="1" t="s">
+      <c r="AB85" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC85" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC85" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD85" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE85" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF85" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>10529</v>
       </c>
@@ -9998,31 +10259,34 @@
         <v>36</v>
       </c>
       <c r="X86" s="1">
+        <v>36</v>
+      </c>
+      <c r="Y86" s="1">
         <v>26</v>
       </c>
-      <c r="Y86" s="1">
-        <v>0</v>
-      </c>
       <c r="Z86" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA86" s="1">
         <v>15</v>
       </c>
-      <c r="AA86" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB86" s="1" t="s">
+      <c r="AB86" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC86" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC86" s="1" t="s">
+      <c r="AD86" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD86" s="1" t="s">
+      <c r="AE86" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE86" s="1" t="s">
+      <c r="AF86" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>10532</v>
       </c>
@@ -10093,31 +10357,34 @@
         <v>25.89</v>
       </c>
       <c r="X87" s="1">
+        <v>25.89</v>
+      </c>
+      <c r="Y87" s="1">
         <v>10</v>
       </c>
-      <c r="Y87" s="1">
-        <v>0</v>
-      </c>
       <c r="Z87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA87" s="1">
         <v>15</v>
       </c>
-      <c r="AA87" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB87" s="1" t="s">
+      <c r="AB87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC87" s="1" t="s">
+      <c r="AD87" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD87" s="1" t="s">
+      <c r="AE87" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AE87" s="1" t="s">
+      <c r="AF87" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>10532</v>
       </c>
@@ -10188,31 +10455,34 @@
         <v>17</v>
       </c>
       <c r="X88" s="1">
+        <v>17</v>
+      </c>
+      <c r="Y88" s="1">
         <v>4</v>
       </c>
-      <c r="Y88" s="1">
+      <c r="Z88" s="1">
         <v>100</v>
       </c>
-      <c r="Z88" s="1">
+      <c r="AA88" s="1">
         <v>20</v>
       </c>
-      <c r="AA88" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB88" s="1" t="s">
+      <c r="AB88" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC88" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC88" s="1" t="s">
+      <c r="AD88" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AD88" s="1" t="s">
+      <c r="AE88" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AE88" s="1" t="s">
+      <c r="AF88" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>10534</v>
       </c>
@@ -10283,31 +10553,34 @@
         <v>25.89</v>
       </c>
       <c r="X89" s="1">
+        <v>25.89</v>
+      </c>
+      <c r="Y89" s="1">
         <v>10</v>
       </c>
-      <c r="Y89" s="1">
-        <v>0</v>
-      </c>
       <c r="Z89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="1">
         <v>15</v>
       </c>
-      <c r="AA89" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB89" s="1" t="s">
+      <c r="AB89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC89" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC89" s="1" t="s">
+      <c r="AD89" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AD89" s="1" t="s">
+      <c r="AE89" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AE89" s="1" t="s">
+      <c r="AF89" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>10534</v>
       </c>
@@ -10378,31 +10651,34 @@
         <v>18.399999999999999</v>
       </c>
       <c r="X90" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Y90" s="1">
         <v>123</v>
       </c>
-      <c r="Y90" s="1">
-        <v>0</v>
-      </c>
       <c r="Z90" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB90" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC90" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC90" s="1" t="s">
+      <c r="AD90" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AD90" s="1" t="s">
+      <c r="AE90" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AE90" s="1" t="s">
+      <c r="AF90" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>10534</v>
       </c>
@@ -10473,31 +10749,34 @@
         <v>7.45</v>
       </c>
       <c r="X91" s="1">
+        <v>7.45</v>
+      </c>
+      <c r="Y91" s="1">
         <v>21</v>
       </c>
-      <c r="Y91" s="1">
-        <v>0</v>
-      </c>
       <c r="Z91" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA91" s="1">
         <v>10</v>
       </c>
-      <c r="AA91" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB91" s="1" t="s">
+      <c r="AB91" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC91" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AC91" s="1" t="s">
+      <c r="AD91" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AD91" s="1" t="s">
+      <c r="AE91" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AE91" s="1" t="s">
+      <c r="AF91" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>10558</v>
       </c>
@@ -10568,31 +10847,34 @@
         <v>9.5</v>
       </c>
       <c r="X92" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="Y92" s="1">
         <v>36</v>
       </c>
-      <c r="Y92" s="1">
-        <v>0</v>
-      </c>
       <c r="Z92" s="1">
         <v>0</v>
       </c>
       <c r="AA92" s="1">
         <v>0</v>
       </c>
-      <c r="AB92" s="1" t="s">
+      <c r="AB92" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC92" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC92" s="1" t="s">
+      <c r="AD92" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="AD92" s="1" t="s">
+      <c r="AE92" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="AE92" s="1" t="s">
+      <c r="AF92" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>10558</v>
       </c>
@@ -10663,31 +10945,34 @@
         <v>53</v>
       </c>
       <c r="X93" s="1">
+        <v>53</v>
+      </c>
+      <c r="Y93" s="1">
         <v>20</v>
       </c>
-      <c r="Y93" s="1">
-        <v>0</v>
-      </c>
       <c r="Z93" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA93" s="1">
         <v>10</v>
       </c>
-      <c r="AA93" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB93" s="1" t="s">
+      <c r="AB93" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC93" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC93" s="1" t="s">
+      <c r="AD93" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD93" s="1" t="s">
+      <c r="AE93" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE93" s="1" t="s">
+      <c r="AF93" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>10558</v>
       </c>
@@ -10758,31 +11043,34 @@
         <v>7</v>
       </c>
       <c r="X94" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y94" s="1">
         <v>38</v>
       </c>
-      <c r="Y94" s="1">
-        <v>0</v>
-      </c>
       <c r="Z94" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA94" s="1">
         <v>25</v>
       </c>
-      <c r="AA94" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB94" s="1" t="s">
+      <c r="AB94" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC94" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC94" s="1" t="s">
+      <c r="AD94" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD94" s="1" t="s">
+      <c r="AE94" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE94" s="1" t="s">
+      <c r="AF94" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>10558</v>
       </c>
@@ -10853,7 +11141,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="X95" s="1">
-        <v>0</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="Y95" s="1">
         <v>0</v>
@@ -10862,22 +11150,25 @@
         <v>0</v>
       </c>
       <c r="AA95" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="1">
         <v>1</v>
       </c>
-      <c r="AB95" s="1" t="s">
+      <c r="AC95" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AC95" s="1" t="s">
+      <c r="AD95" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD95" s="1" t="s">
+      <c r="AE95" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE95" s="1" t="s">
+      <c r="AF95" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>10558</v>
       </c>
@@ -10948,31 +11239,34 @@
         <v>15</v>
       </c>
       <c r="X96" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y96" s="1">
         <v>101</v>
       </c>
-      <c r="Y96" s="1">
-        <v>0</v>
-      </c>
       <c r="Z96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA96" s="1">
         <v>5</v>
       </c>
-      <c r="AA96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB96" s="1" t="s">
+      <c r="AB96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC96" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC96" s="1" t="s">
+      <c r="AD96" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD96" s="1" t="s">
+      <c r="AE96" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AE96" s="1" t="s">
+      <c r="AF96" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>10596</v>
       </c>
@@ -11043,31 +11337,34 @@
         <v>38</v>
       </c>
       <c r="X97" s="1">
+        <v>38</v>
+      </c>
+      <c r="Y97" s="1">
         <v>21</v>
       </c>
-      <c r="Y97" s="1">
+      <c r="Z97" s="1">
         <v>10</v>
       </c>
-      <c r="Z97" s="1">
-        <v>30</v>
-      </c>
       <c r="AA97" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB97" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB97" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC97" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC97" s="1" t="s">
+      <c r="AD97" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AD97" s="1" t="s">
+      <c r="AE97" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AE97" s="1" t="s">
+      <c r="AF97" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>10596</v>
       </c>
@@ -11138,31 +11435,34 @@
         <v>43.9</v>
       </c>
       <c r="X98" s="1">
+        <v>43.9</v>
+      </c>
+      <c r="Y98" s="1">
         <v>24</v>
       </c>
-      <c r="Y98" s="1">
-        <v>0</v>
-      </c>
       <c r="Z98" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA98" s="1">
         <v>5</v>
       </c>
-      <c r="AA98" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB98" s="1" t="s">
+      <c r="AB98" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC98" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="AC98" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="AD98" s="1" t="s">
         <v>304</v>
       </c>
       <c r="AE98" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF98" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>10596</v>
       </c>
@@ -11233,31 +11533,34 @@
         <v>7.75</v>
       </c>
       <c r="X99" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="Y99" s="1">
         <v>125</v>
       </c>
-      <c r="Y99" s="1">
-        <v>0</v>
-      </c>
       <c r="Z99" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA99" s="1">
         <v>25</v>
       </c>
-      <c r="AA99" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB99" s="1" t="s">
+      <c r="AB99" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC99" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC99" s="1" t="s">
+      <c r="AD99" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD99" s="1" t="s">
+      <c r="AE99" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE99" s="1" t="s">
+      <c r="AF99" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>10620</v>
       </c>
@@ -11328,31 +11631,34 @@
         <v>4.5</v>
       </c>
       <c r="X100" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Y100" s="1">
         <v>20</v>
       </c>
-      <c r="Y100" s="1">
-        <v>0</v>
-      </c>
       <c r="Z100" s="1">
         <v>0</v>
       </c>
       <c r="AA100" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="1">
         <v>1</v>
       </c>
-      <c r="AB100" s="1" t="s">
+      <c r="AC100" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AC100" s="1" t="s">
+      <c r="AD100" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AD100" s="1" t="s">
+      <c r="AE100" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="AE100" s="1" t="s">
+      <c r="AF100" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>10620</v>
       </c>
@@ -11423,31 +11729,34 @@
         <v>7</v>
       </c>
       <c r="X101" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y101" s="1">
         <v>38</v>
       </c>
-      <c r="Y101" s="1">
-        <v>0</v>
-      </c>
       <c r="Z101" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA101" s="1">
         <v>25</v>
       </c>
-      <c r="AA101" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB101" s="1" t="s">
+      <c r="AB101" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC101" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC101" s="1" t="s">
+      <c r="AD101" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD101" s="1" t="s">
+      <c r="AE101" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE101" s="1" t="s">
+      <c r="AF101" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>10621</v>
       </c>
@@ -11518,31 +11827,34 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="X102" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Y102" s="1">
         <v>25</v>
       </c>
-      <c r="Y102" s="1">
-        <v>0</v>
-      </c>
       <c r="Z102" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA102" s="1">
         <v>5</v>
       </c>
-      <c r="AA102" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB102" s="1" t="s">
+      <c r="AB102" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC102" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC102" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="AD102" s="1" t="s">
         <v>305</v>
       </c>
       <c r="AE102" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF102" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>10624</v>
       </c>
@@ -11613,31 +11925,34 @@
         <v>45.6</v>
       </c>
       <c r="X103" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="Y103" s="1">
         <v>26</v>
       </c>
-      <c r="Y103" s="1">
-        <v>0</v>
-      </c>
       <c r="Z103" s="1">
         <v>0</v>
       </c>
       <c r="AA103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB103" s="1">
         <v>1</v>
       </c>
-      <c r="AB103" s="1" t="s">
+      <c r="AC103" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC103" s="1" t="s">
+      <c r="AD103" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD103" s="1" t="s">
+      <c r="AE103" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE103" s="1" t="s">
+      <c r="AF103" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>10624</v>
       </c>
@@ -11708,7 +12023,7 @@
         <v>123.79</v>
       </c>
       <c r="X104" s="1">
-        <v>0</v>
+        <v>123.79</v>
       </c>
       <c r="Y104" s="1">
         <v>0</v>
@@ -11717,22 +12032,25 @@
         <v>0</v>
       </c>
       <c r="AA104" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB104" s="1">
         <v>1</v>
       </c>
-      <c r="AB104" s="1" t="s">
+      <c r="AC104" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AC104" s="1" t="s">
+      <c r="AD104" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AD104" s="1" t="s">
+      <c r="AE104" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AE104" s="1" t="s">
+      <c r="AF104" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>10624</v>
       </c>
@@ -11803,31 +12121,34 @@
         <v>19.45</v>
       </c>
       <c r="X105" s="1">
+        <v>19.45</v>
+      </c>
+      <c r="Y105" s="1">
         <v>27</v>
       </c>
-      <c r="Y105" s="1">
-        <v>0</v>
-      </c>
       <c r="Z105" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA105" s="1">
         <v>15</v>
       </c>
-      <c r="AA105" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB105" s="1" t="s">
+      <c r="AB105" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC105" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC105" s="1" t="s">
+      <c r="AD105" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AD105" s="1" t="s">
+      <c r="AE105" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AE105" s="1" t="s">
+      <c r="AF105" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>10625</v>
       </c>
@@ -11898,31 +12219,34 @@
         <v>23.25</v>
       </c>
       <c r="X106" s="1">
+        <v>23.25</v>
+      </c>
+      <c r="Y106" s="1">
         <v>35</v>
       </c>
-      <c r="Y106" s="1">
-        <v>0</v>
-      </c>
       <c r="Z106" s="1">
         <v>0</v>
       </c>
       <c r="AA106" s="1">
         <v>0</v>
       </c>
-      <c r="AB106" s="1" t="s">
+      <c r="AB106" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC106" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC106" s="1" t="s">
+      <c r="AD106" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AD106" s="1" t="s">
+      <c r="AE106" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AE106" s="1" t="s">
+      <c r="AF106" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>10625</v>
       </c>
@@ -11993,31 +12317,34 @@
         <v>14</v>
       </c>
       <c r="X107" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y107" s="1">
         <v>26</v>
       </c>
-      <c r="Y107" s="1">
-        <v>0</v>
-      </c>
       <c r="Z107" s="1">
         <v>0</v>
       </c>
       <c r="AA107" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB107" s="1">
         <v>1</v>
       </c>
-      <c r="AB107" s="1" t="s">
+      <c r="AC107" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AC107" s="1" t="s">
+      <c r="AD107" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AD107" s="1" t="s">
+      <c r="AE107" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AE107" s="1" t="s">
+      <c r="AF107" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>10625</v>
       </c>
@@ -12088,32 +12415,35 @@
         <v>34</v>
       </c>
       <c r="X108" s="1">
+        <v>34</v>
+      </c>
+      <c r="Y108" s="1">
         <v>19</v>
       </c>
-      <c r="Y108" s="1">
-        <v>0</v>
-      </c>
       <c r="Z108" s="1">
         <v>0</v>
       </c>
       <c r="AA108" s="1">
         <v>0</v>
       </c>
-      <c r="AB108" s="1" t="s">
+      <c r="AB108" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC108" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC108" s="1" t="s">
+      <c r="AD108" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AD108" s="1" t="s">
+      <c r="AE108" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AE108" s="1" t="s">
+      <c r="AF108" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AF108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>